<commit_message>
Implemented Unit Testing Cases
</commit_message>
<xml_diff>
--- a/data/Operations_Data.xlsx
+++ b/data/Operations_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\MSTS_FJSP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78C7E0F-7D2D-45D2-B0E8-CA6C9B498C6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FC27F6-88EF-4DD0-B0BA-0BE5A4EE98D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{1D379F6F-46A7-404F-89DA-62600F8E0E9F}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
   <si>
     <t>Job</t>
   </si>
@@ -521,7 +521,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,15 +605,15 @@
       </c>
       <c r="H2" s="2" cm="1">
         <f t="array" aca="1" ref="H2" ca="1">_xlfn.IFS( ((D2/(E2*(F2/(PI()*G2))))*60)&gt;1000, MROUND(RANDBETWEEN(800,1000),10), ((D2/(E2*(F2/(PI()*G2))))*60)&lt;100, MROUND(RANDBETWEEN(100,200),10), ((D2/(E2*(F2/(PI()*G2))))*60)&gt;100, MROUND((D2/(E2*(F2/(PI()*G2))))*60,10))</f>
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="I2" s="2" cm="1">
         <f t="array" aca="1" ref="I2" ca="1">_xlfn.IFS(C2="Milling",MROUND(RANDBETWEEN(300,500), 10), C2="Turning",MROUND(RANDBETWEEN(200,400), 10), C2="Drilling",MROUND(RANDBETWEEN(50,100), 10), C2="Grinding",MROUND(RANDBETWEEN(50,100), 10), C2="Boring",MROUND(RANDBETWEEN(50,100), 10), C2="Grooving",MROUND(RANDBETWEEN(100,250), 10), C2="Broaching",MROUND(RANDBETWEEN(200,400), 10), C2="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>420</v>
+        <v>400</v>
       </c>
       <c r="J2" s="2">
         <f ca="1">H2+I2</f>
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
@@ -652,11 +652,11 @@
       </c>
       <c r="I3" s="2" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">_xlfn.IFS(C3="Milling",MROUND(RANDBETWEEN(300,500), 10), C3="Turning",MROUND(RANDBETWEEN(200,400), 10), C3="Drilling",MROUND(RANDBETWEEN(50,100), 10), C3="Grinding",MROUND(RANDBETWEEN(50,100), 10), C3="Boring",MROUND(RANDBETWEEN(50,100), 10), C3="Grooving",MROUND(RANDBETWEEN(100,250), 10), C3="Broaching",MROUND(RANDBETWEEN(200,400), 10), C3="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ref="J3:J11" ca="1" si="0">H3+I3</f>
-        <v>1020</v>
+        <v>1010</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>11</v>
@@ -697,11 +697,11 @@
       </c>
       <c r="I4" s="2" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">_xlfn.IFS(C4="Milling",MROUND(RANDBETWEEN(300,500), 10), C4="Turning",MROUND(RANDBETWEEN(200,400), 10), C4="Drilling",MROUND(RANDBETWEEN(50,100), 10), C4="Grinding",MROUND(RANDBETWEEN(50,100), 10), C4="Boring",MROUND(RANDBETWEEN(50,100), 10), C4="Grooving",MROUND(RANDBETWEEN(100,250), 10), C4="Broaching",MROUND(RANDBETWEEN(200,400), 10), C4="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>410</v>
+        <v>390</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>12</v>
@@ -742,11 +742,11 @@
       </c>
       <c r="I5" s="2" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">_xlfn.IFS(C5="Milling",MROUND(RANDBETWEEN(300,500), 10), C5="Turning",MROUND(RANDBETWEEN(200,400), 10), C5="Drilling",MROUND(RANDBETWEEN(50,100), 10), C5="Grinding",MROUND(RANDBETWEEN(50,100), 10), C5="Boring",MROUND(RANDBETWEEN(50,100), 10), C5="Grooving",MROUND(RANDBETWEEN(100,250), 10), C5="Broaching",MROUND(RANDBETWEEN(200,400), 10), C5="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>340</v>
+        <v>270</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1010</v>
+        <v>940</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>12</v>
@@ -828,22 +828,20 @@
       </c>
       <c r="H7" s="2" cm="1">
         <f t="array" aca="1" ref="H7" ca="1">_xlfn.IFS( ((D7/(E7*(F7/(PI()*G7))))*60)&gt;1000, MROUND(RANDBETWEEN(800,1000),10), ((D7/(E7*(F7/(PI()*G7))))*60)&lt;100, MROUND(RANDBETWEEN(100,200),10), ((D7/(E7*(F7/(PI()*G7))))*60)&gt;100, MROUND((D7/(E7*(F7/(PI()*G7))))*60,10))</f>
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="I7" s="2" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_xlfn.IFS(C7="Milling",MROUND(RANDBETWEEN(300,500), 10), C7="Turning",MROUND(RANDBETWEEN(200,400), 10), C7="Drilling",MROUND(RANDBETWEEN(50,100), 10), C7="Grinding",MROUND(RANDBETWEEN(50,100), 10), C7="Boring",MROUND(RANDBETWEEN(50,100), 10), C7="Grooving",MROUND(RANDBETWEEN(100,250), 10), C7="Broaching",MROUND(RANDBETWEEN(200,400), 10), C7="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="L7" s="2"/>
       <c r="M7" s="1" t="s">
         <v>18</v>
       </c>
@@ -877,11 +875,11 @@
       </c>
       <c r="I8" s="2" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_xlfn.IFS(C8="Milling",MROUND(RANDBETWEEN(300,500), 10), C8="Turning",MROUND(RANDBETWEEN(200,400), 10), C8="Drilling",MROUND(RANDBETWEEN(50,100), 10), C8="Grinding",MROUND(RANDBETWEEN(50,100), 10), C8="Boring",MROUND(RANDBETWEEN(50,100), 10), C8="Grooving",MROUND(RANDBETWEEN(100,250), 10), C8="Broaching",MROUND(RANDBETWEEN(200,400), 10), C8="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>470</v>
+        <v>350</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>580</v>
+        <v>460</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="s">
@@ -920,11 +918,11 @@
       </c>
       <c r="I9" s="2" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_xlfn.IFS(C9="Milling",MROUND(RANDBETWEEN(300,500), 10), C9="Turning",MROUND(RANDBETWEEN(200,400), 10), C9="Drilling",MROUND(RANDBETWEEN(50,100), 10), C9="Grinding",MROUND(RANDBETWEEN(50,100), 10), C9="Boring",MROUND(RANDBETWEEN(50,100), 10), C9="Grooving",MROUND(RANDBETWEEN(100,250), 10), C9="Broaching",MROUND(RANDBETWEEN(200,400), 10), C9="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>250</v>
+        <v>280</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>690</v>
+        <v>720</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>27</v>
@@ -965,11 +963,11 @@
       </c>
       <c r="I10" s="2" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">_xlfn.IFS(C10="Milling",MROUND(RANDBETWEEN(300,500), 10), C10="Turning",MROUND(RANDBETWEEN(200,400), 10), C10="Drilling",MROUND(RANDBETWEEN(50,100), 10), C10="Grinding",MROUND(RANDBETWEEN(50,100), 10), C10="Boring",MROUND(RANDBETWEEN(50,100), 10), C10="Grooving",MROUND(RANDBETWEEN(100,250), 10), C10="Broaching",MROUND(RANDBETWEEN(200,400), 10), C10="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>27</v>
@@ -1010,11 +1008,11 @@
       </c>
       <c r="I11" s="2" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_xlfn.IFS(C11="Milling",MROUND(RANDBETWEEN(300,500), 10), C11="Turning",MROUND(RANDBETWEEN(200,400), 10), C11="Drilling",MROUND(RANDBETWEEN(50,100), 10), C11="Grinding",MROUND(RANDBETWEEN(50,100), 10), C11="Boring",MROUND(RANDBETWEEN(50,100), 10), C11="Grooving",MROUND(RANDBETWEEN(100,250), 10), C11="Broaching",MROUND(RANDBETWEEN(200,400), 10), C11="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>390</v>
+        <v>360</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>490</v>
+        <v>460</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Begin ShortestPath Algorithm and introduce dealing with parallel operations
</commit_message>
<xml_diff>
--- a/data/Operations_Data.xlsx
+++ b/data/Operations_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\MSTS_FJSP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FC27F6-88EF-4DD0-B0BA-0BE5A4EE98D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEABA620-E6E9-492D-B838-4DCF6DFB5C81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{1D379F6F-46A7-404F-89DA-62600F8E0E9F}"/>
   </bookViews>
@@ -157,13 +157,13 @@
     <t>Succ_Op</t>
   </si>
   <si>
-    <t>O13, O14</t>
-  </si>
-  <si>
-    <t>O14, O15</t>
-  </si>
-  <si>
-    <t>O22, O23</t>
+    <t>O13,O14</t>
+  </si>
+  <si>
+    <t>O14,O15</t>
+  </si>
+  <si>
+    <t>O22,O23</t>
   </si>
 </sst>
 </file>
@@ -521,7 +521,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,15 +605,15 @@
       </c>
       <c r="H2" s="2" cm="1">
         <f t="array" aca="1" ref="H2" ca="1">_xlfn.IFS( ((D2/(E2*(F2/(PI()*G2))))*60)&gt;1000, MROUND(RANDBETWEEN(800,1000),10), ((D2/(E2*(F2/(PI()*G2))))*60)&lt;100, MROUND(RANDBETWEEN(100,200),10), ((D2/(E2*(F2/(PI()*G2))))*60)&gt;100, MROUND((D2/(E2*(F2/(PI()*G2))))*60,10))</f>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="I2" s="2" cm="1">
         <f t="array" aca="1" ref="I2" ca="1">_xlfn.IFS(C2="Milling",MROUND(RANDBETWEEN(300,500), 10), C2="Turning",MROUND(RANDBETWEEN(200,400), 10), C2="Drilling",MROUND(RANDBETWEEN(50,100), 10), C2="Grinding",MROUND(RANDBETWEEN(50,100), 10), C2="Boring",MROUND(RANDBETWEEN(50,100), 10), C2="Grooving",MROUND(RANDBETWEEN(100,250), 10), C2="Broaching",MROUND(RANDBETWEEN(200,400), 10), C2="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="J2" s="2">
         <f ca="1">H2+I2</f>
-        <v>540</v>
+        <v>570</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
@@ -652,11 +652,11 @@
       </c>
       <c r="I3" s="2" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">_xlfn.IFS(C3="Milling",MROUND(RANDBETWEEN(300,500), 10), C3="Turning",MROUND(RANDBETWEEN(200,400), 10), C3="Drilling",MROUND(RANDBETWEEN(50,100), 10), C3="Grinding",MROUND(RANDBETWEEN(50,100), 10), C3="Boring",MROUND(RANDBETWEEN(50,100), 10), C3="Grooving",MROUND(RANDBETWEEN(100,250), 10), C3="Broaching",MROUND(RANDBETWEEN(200,400), 10), C3="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>340</v>
+        <v>230</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ref="J3:J11" ca="1" si="0">H3+I3</f>
-        <v>1010</v>
+        <v>900</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>11</v>
@@ -697,11 +697,11 @@
       </c>
       <c r="I4" s="2" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">_xlfn.IFS(C4="Milling",MROUND(RANDBETWEEN(300,500), 10), C4="Turning",MROUND(RANDBETWEEN(200,400), 10), C4="Drilling",MROUND(RANDBETWEEN(50,100), 10), C4="Grinding",MROUND(RANDBETWEEN(50,100), 10), C4="Boring",MROUND(RANDBETWEEN(50,100), 10), C4="Grooving",MROUND(RANDBETWEEN(100,250), 10), C4="Broaching",MROUND(RANDBETWEEN(200,400), 10), C4="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>210</v>
+        <v>370</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>390</v>
+        <v>550</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>12</v>
@@ -742,11 +742,11 @@
       </c>
       <c r="I5" s="2" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">_xlfn.IFS(C5="Milling",MROUND(RANDBETWEEN(300,500), 10), C5="Turning",MROUND(RANDBETWEEN(200,400), 10), C5="Drilling",MROUND(RANDBETWEEN(50,100), 10), C5="Grinding",MROUND(RANDBETWEEN(50,100), 10), C5="Boring",MROUND(RANDBETWEEN(50,100), 10), C5="Grooving",MROUND(RANDBETWEEN(100,250), 10), C5="Broaching",MROUND(RANDBETWEEN(200,400), 10), C5="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>940</v>
+        <v>950</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>12</v>
@@ -787,11 +787,11 @@
       </c>
       <c r="I6" s="2" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">_xlfn.IFS(C6="Milling",MROUND(RANDBETWEEN(300,500), 10), C6="Turning",MROUND(RANDBETWEEN(200,400), 10), C6="Drilling",MROUND(RANDBETWEEN(50,100), 10), C6="Grinding",MROUND(RANDBETWEEN(50,100), 10), C6="Boring",MROUND(RANDBETWEEN(50,100), 10), C6="Grooving",MROUND(RANDBETWEEN(100,250), 10), C6="Broaching",MROUND(RANDBETWEEN(200,400), 10), C6="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>440</v>
+        <v>470</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>13</v>
@@ -828,7 +828,7 @@
       </c>
       <c r="H7" s="2" cm="1">
         <f t="array" aca="1" ref="H7" ca="1">_xlfn.IFS( ((D7/(E7*(F7/(PI()*G7))))*60)&gt;1000, MROUND(RANDBETWEEN(800,1000),10), ((D7/(E7*(F7/(PI()*G7))))*60)&lt;100, MROUND(RANDBETWEEN(100,200),10), ((D7/(E7*(F7/(PI()*G7))))*60)&gt;100, MROUND((D7/(E7*(F7/(PI()*G7))))*60,10))</f>
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="I7" s="2" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_xlfn.IFS(C7="Milling",MROUND(RANDBETWEEN(300,500), 10), C7="Turning",MROUND(RANDBETWEEN(200,400), 10), C7="Drilling",MROUND(RANDBETWEEN(50,100), 10), C7="Grinding",MROUND(RANDBETWEEN(50,100), 10), C7="Boring",MROUND(RANDBETWEEN(50,100), 10), C7="Grooving",MROUND(RANDBETWEEN(100,250), 10), C7="Broaching",MROUND(RANDBETWEEN(200,400), 10), C7="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
@@ -836,7 +836,7 @@
       </c>
       <c r="J7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>210</v>
+        <v>160</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>34</v>
@@ -875,11 +875,11 @@
       </c>
       <c r="I8" s="2" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_xlfn.IFS(C8="Milling",MROUND(RANDBETWEEN(300,500), 10), C8="Turning",MROUND(RANDBETWEEN(200,400), 10), C8="Drilling",MROUND(RANDBETWEEN(50,100), 10), C8="Grinding",MROUND(RANDBETWEEN(50,100), 10), C8="Boring",MROUND(RANDBETWEEN(50,100), 10), C8="Grooving",MROUND(RANDBETWEEN(100,250), 10), C8="Broaching",MROUND(RANDBETWEEN(200,400), 10), C8="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>350</v>
+        <v>370</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>460</v>
+        <v>480</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="s">
@@ -918,11 +918,11 @@
       </c>
       <c r="I9" s="2" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_xlfn.IFS(C9="Milling",MROUND(RANDBETWEEN(300,500), 10), C9="Turning",MROUND(RANDBETWEEN(200,400), 10), C9="Drilling",MROUND(RANDBETWEEN(50,100), 10), C9="Grinding",MROUND(RANDBETWEEN(50,100), 10), C9="Boring",MROUND(RANDBETWEEN(50,100), 10), C9="Grooving",MROUND(RANDBETWEEN(100,250), 10), C9="Broaching",MROUND(RANDBETWEEN(200,400), 10), C9="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>280</v>
+        <v>320</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>720</v>
+        <v>760</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>27</v>
@@ -963,11 +963,11 @@
       </c>
       <c r="I10" s="2" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">_xlfn.IFS(C10="Milling",MROUND(RANDBETWEEN(300,500), 10), C10="Turning",MROUND(RANDBETWEEN(200,400), 10), C10="Drilling",MROUND(RANDBETWEEN(50,100), 10), C10="Grinding",MROUND(RANDBETWEEN(50,100), 10), C10="Boring",MROUND(RANDBETWEEN(50,100), 10), C10="Grooving",MROUND(RANDBETWEEN(100,250), 10), C10="Broaching",MROUND(RANDBETWEEN(200,400), 10), C10="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>590</v>
+        <v>560</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>27</v>
@@ -1008,11 +1008,11 @@
       </c>
       <c r="I11" s="2" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_xlfn.IFS(C11="Milling",MROUND(RANDBETWEEN(300,500), 10), C11="Turning",MROUND(RANDBETWEEN(200,400), 10), C11="Drilling",MROUND(RANDBETWEEN(50,100), 10), C11="Grinding",MROUND(RANDBETWEEN(50,100), 10), C11="Boring",MROUND(RANDBETWEEN(50,100), 10), C11="Grooving",MROUND(RANDBETWEEN(100,250), 10), C11="Broaching",MROUND(RANDBETWEEN(200,400), 10), C11="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>360</v>
+        <v>460</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>460</v>
+        <v>560</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Completed Shortest Path Algorithm
</commit_message>
<xml_diff>
--- a/data/Operations_Data.xlsx
+++ b/data/Operations_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\MSTS_FJSP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEABA620-E6E9-492D-B838-4DCF6DFB5C81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC06297B-3115-4D1D-9B64-46F50E530F3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{1D379F6F-46A7-404F-89DA-62600F8E0E9F}"/>
   </bookViews>
@@ -160,10 +160,10 @@
     <t>O13,O14</t>
   </si>
   <si>
-    <t>O14,O15</t>
-  </si>
-  <si>
     <t>O22,O23</t>
+  </si>
+  <si>
+    <t>O15,O14</t>
   </si>
 </sst>
 </file>
@@ -521,7 +521,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,15 +605,15 @@
       </c>
       <c r="H2" s="2" cm="1">
         <f t="array" aca="1" ref="H2" ca="1">_xlfn.IFS( ((D2/(E2*(F2/(PI()*G2))))*60)&gt;1000, MROUND(RANDBETWEEN(800,1000),10), ((D2/(E2*(F2/(PI()*G2))))*60)&lt;100, MROUND(RANDBETWEEN(100,200),10), ((D2/(E2*(F2/(PI()*G2))))*60)&gt;100, MROUND((D2/(E2*(F2/(PI()*G2))))*60,10))</f>
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="I2" s="2" cm="1">
         <f t="array" aca="1" ref="I2" ca="1">_xlfn.IFS(C2="Milling",MROUND(RANDBETWEEN(300,500), 10), C2="Turning",MROUND(RANDBETWEEN(200,400), 10), C2="Drilling",MROUND(RANDBETWEEN(50,100), 10), C2="Grinding",MROUND(RANDBETWEEN(50,100), 10), C2="Boring",MROUND(RANDBETWEEN(50,100), 10), C2="Grooving",MROUND(RANDBETWEEN(100,250), 10), C2="Broaching",MROUND(RANDBETWEEN(200,400), 10), C2="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>410</v>
+        <v>480</v>
       </c>
       <c r="J2" s="2">
         <f ca="1">H2+I2</f>
-        <v>570</v>
+        <v>650</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
@@ -652,11 +652,11 @@
       </c>
       <c r="I3" s="2" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">_xlfn.IFS(C3="Milling",MROUND(RANDBETWEEN(300,500), 10), C3="Turning",MROUND(RANDBETWEEN(200,400), 10), C3="Drilling",MROUND(RANDBETWEEN(50,100), 10), C3="Grinding",MROUND(RANDBETWEEN(50,100), 10), C3="Boring",MROUND(RANDBETWEEN(50,100), 10), C3="Grooving",MROUND(RANDBETWEEN(100,250), 10), C3="Broaching",MROUND(RANDBETWEEN(200,400), 10), C3="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>230</v>
+        <v>370</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ref="J3:J11" ca="1" si="0">H3+I3</f>
-        <v>900</v>
+        <v>1040</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>11</v>
@@ -697,11 +697,11 @@
       </c>
       <c r="I4" s="2" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">_xlfn.IFS(C4="Milling",MROUND(RANDBETWEEN(300,500), 10), C4="Turning",MROUND(RANDBETWEEN(200,400), 10), C4="Drilling",MROUND(RANDBETWEEN(50,100), 10), C4="Grinding",MROUND(RANDBETWEEN(50,100), 10), C4="Boring",MROUND(RANDBETWEEN(50,100), 10), C4="Grooving",MROUND(RANDBETWEEN(100,250), 10), C4="Broaching",MROUND(RANDBETWEEN(200,400), 10), C4="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>370</v>
+        <v>350</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>550</v>
+        <v>530</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>12</v>
@@ -742,11 +742,11 @@
       </c>
       <c r="I5" s="2" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">_xlfn.IFS(C5="Milling",MROUND(RANDBETWEEN(300,500), 10), C5="Turning",MROUND(RANDBETWEEN(200,400), 10), C5="Drilling",MROUND(RANDBETWEEN(50,100), 10), C5="Grinding",MROUND(RANDBETWEEN(50,100), 10), C5="Boring",MROUND(RANDBETWEEN(50,100), 10), C5="Grooving",MROUND(RANDBETWEEN(100,250), 10), C5="Broaching",MROUND(RANDBETWEEN(200,400), 10), C5="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>280</v>
+        <v>220</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>950</v>
+        <v>890</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>12</v>
@@ -787,11 +787,11 @@
       </c>
       <c r="I6" s="2" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">_xlfn.IFS(C6="Milling",MROUND(RANDBETWEEN(300,500), 10), C6="Turning",MROUND(RANDBETWEEN(200,400), 10), C6="Drilling",MROUND(RANDBETWEEN(50,100), 10), C6="Grinding",MROUND(RANDBETWEEN(50,100), 10), C6="Boring",MROUND(RANDBETWEEN(50,100), 10), C6="Grooving",MROUND(RANDBETWEEN(100,250), 10), C6="Broaching",MROUND(RANDBETWEEN(200,400), 10), C6="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>470</v>
+        <v>440</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>13</v>
@@ -828,7 +828,7 @@
       </c>
       <c r="H7" s="2" cm="1">
         <f t="array" aca="1" ref="H7" ca="1">_xlfn.IFS( ((D7/(E7*(F7/(PI()*G7))))*60)&gt;1000, MROUND(RANDBETWEEN(800,1000),10), ((D7/(E7*(F7/(PI()*G7))))*60)&lt;100, MROUND(RANDBETWEEN(100,200),10), ((D7/(E7*(F7/(PI()*G7))))*60)&gt;100, MROUND((D7/(E7*(F7/(PI()*G7))))*60,10))</f>
-        <v>100</v>
+        <v>190</v>
       </c>
       <c r="I7" s="2" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_xlfn.IFS(C7="Milling",MROUND(RANDBETWEEN(300,500), 10), C7="Turning",MROUND(RANDBETWEEN(200,400), 10), C7="Drilling",MROUND(RANDBETWEEN(50,100), 10), C7="Grinding",MROUND(RANDBETWEEN(50,100), 10), C7="Boring",MROUND(RANDBETWEEN(50,100), 10), C7="Grooving",MROUND(RANDBETWEEN(100,250), 10), C7="Broaching",MROUND(RANDBETWEEN(200,400), 10), C7="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
@@ -836,10 +836,10 @@
       </c>
       <c r="J7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>160</v>
+        <v>250</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="1" t="s">
@@ -875,15 +875,15 @@
       </c>
       <c r="I8" s="2" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_xlfn.IFS(C8="Milling",MROUND(RANDBETWEEN(300,500), 10), C8="Turning",MROUND(RANDBETWEEN(200,400), 10), C8="Drilling",MROUND(RANDBETWEEN(50,100), 10), C8="Grinding",MROUND(RANDBETWEEN(50,100), 10), C8="Boring",MROUND(RANDBETWEEN(50,100), 10), C8="Grooving",MROUND(RANDBETWEEN(100,250), 10), C8="Broaching",MROUND(RANDBETWEEN(200,400), 10), C8="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>370</v>
+        <v>450</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>480</v>
+        <v>560</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>18</v>
@@ -918,11 +918,11 @@
       </c>
       <c r="I9" s="2" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_xlfn.IFS(C9="Milling",MROUND(RANDBETWEEN(300,500), 10), C9="Turning",MROUND(RANDBETWEEN(200,400), 10), C9="Drilling",MROUND(RANDBETWEEN(50,100), 10), C9="Grinding",MROUND(RANDBETWEEN(50,100), 10), C9="Boring",MROUND(RANDBETWEEN(50,100), 10), C9="Grooving",MROUND(RANDBETWEEN(100,250), 10), C9="Broaching",MROUND(RANDBETWEEN(200,400), 10), C9="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>760</v>
+        <v>770</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>27</v>
@@ -963,11 +963,11 @@
       </c>
       <c r="I10" s="2" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">_xlfn.IFS(C10="Milling",MROUND(RANDBETWEEN(300,500), 10), C10="Turning",MROUND(RANDBETWEEN(200,400), 10), C10="Drilling",MROUND(RANDBETWEEN(50,100), 10), C10="Grinding",MROUND(RANDBETWEEN(50,100), 10), C10="Boring",MROUND(RANDBETWEEN(50,100), 10), C10="Grooving",MROUND(RANDBETWEEN(100,250), 10), C10="Broaching",MROUND(RANDBETWEEN(200,400), 10), C10="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>560</v>
+        <v>550</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>27</v>
@@ -1008,14 +1008,14 @@
       </c>
       <c r="I11" s="2" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_xlfn.IFS(C11="Milling",MROUND(RANDBETWEEN(300,500), 10), C11="Turning",MROUND(RANDBETWEEN(200,400), 10), C11="Drilling",MROUND(RANDBETWEEN(50,100), 10), C11="Grinding",MROUND(RANDBETWEEN(50,100), 10), C11="Boring",MROUND(RANDBETWEEN(50,100), 10), C11="Grooving",MROUND(RANDBETWEEN(100,250), 10), C11="Broaching",MROUND(RANDBETWEEN(200,400), 10), C11="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>460</v>
+        <v>500</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>560</v>
+        <v>600</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="1" t="s">

</xml_diff>

<commit_message>
Fixed Parallel Pre operation edge case and started operation scheduling algorithm
</commit_message>
<xml_diff>
--- a/data/Operations_Data.xlsx
+++ b/data/Operations_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\MSTS_FJSP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC06297B-3115-4D1D-9B64-46F50E530F3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F4F146-5023-47D8-BFA9-60C8A6416C2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{1D379F6F-46A7-404F-89DA-62600F8E0E9F}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
   <si>
     <t>Job</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>O15,O14</t>
+  </si>
+  <si>
+    <t>Finishing_time</t>
   </si>
 </sst>
 </file>
@@ -518,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4E1EF2B-2F89-413B-9BEE-B2178CC6644E}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,7 +540,7 @@
     <col min="11" max="12" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -580,8 +583,11 @@
       <c r="N1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -605,15 +611,15 @@
       </c>
       <c r="H2" s="2" cm="1">
         <f t="array" aca="1" ref="H2" ca="1">_xlfn.IFS( ((D2/(E2*(F2/(PI()*G2))))*60)&gt;1000, MROUND(RANDBETWEEN(800,1000),10), ((D2/(E2*(F2/(PI()*G2))))*60)&lt;100, MROUND(RANDBETWEEN(100,200),10), ((D2/(E2*(F2/(PI()*G2))))*60)&gt;100, MROUND((D2/(E2*(F2/(PI()*G2))))*60,10))</f>
-        <v>170</v>
+        <v>130</v>
       </c>
       <c r="I2" s="2" cm="1">
         <f t="array" aca="1" ref="I2" ca="1">_xlfn.IFS(C2="Milling",MROUND(RANDBETWEEN(300,500), 10), C2="Turning",MROUND(RANDBETWEEN(200,400), 10), C2="Drilling",MROUND(RANDBETWEEN(50,100), 10), C2="Grinding",MROUND(RANDBETWEEN(50,100), 10), C2="Boring",MROUND(RANDBETWEEN(50,100), 10), C2="Grooving",MROUND(RANDBETWEEN(100,250), 10), C2="Broaching",MROUND(RANDBETWEEN(200,400), 10), C2="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>480</v>
+        <v>320</v>
       </c>
       <c r="J2" s="2">
         <f ca="1">H2+I2</f>
-        <v>650</v>
+        <v>450</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
@@ -623,8 +629,11 @@
         <v>18</v>
       </c>
       <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -652,11 +661,11 @@
       </c>
       <c r="I3" s="2" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">_xlfn.IFS(C3="Milling",MROUND(RANDBETWEEN(300,500), 10), C3="Turning",MROUND(RANDBETWEEN(200,400), 10), C3="Drilling",MROUND(RANDBETWEEN(50,100), 10), C3="Grinding",MROUND(RANDBETWEEN(50,100), 10), C3="Boring",MROUND(RANDBETWEEN(50,100), 10), C3="Grooving",MROUND(RANDBETWEEN(100,250), 10), C3="Broaching",MROUND(RANDBETWEEN(200,400), 10), C3="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>370</v>
+        <v>330</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ref="J3:J11" ca="1" si="0">H3+I3</f>
-        <v>1040</v>
+        <v>1000</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>11</v>
@@ -668,8 +677,11 @@
         <v>18</v>
       </c>
       <c r="N3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -697,11 +709,11 @@
       </c>
       <c r="I4" s="2" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">_xlfn.IFS(C4="Milling",MROUND(RANDBETWEEN(300,500), 10), C4="Turning",MROUND(RANDBETWEEN(200,400), 10), C4="Drilling",MROUND(RANDBETWEEN(50,100), 10), C4="Grinding",MROUND(RANDBETWEEN(50,100), 10), C4="Boring",MROUND(RANDBETWEEN(50,100), 10), C4="Grooving",MROUND(RANDBETWEEN(100,250), 10), C4="Broaching",MROUND(RANDBETWEEN(200,400), 10), C4="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>350</v>
+        <v>290</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>530</v>
+        <v>470</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>12</v>
@@ -713,8 +725,11 @@
         <v>17</v>
       </c>
       <c r="N4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -742,11 +757,11 @@
       </c>
       <c r="I5" s="2" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">_xlfn.IFS(C5="Milling",MROUND(RANDBETWEEN(300,500), 10), C5="Turning",MROUND(RANDBETWEEN(200,400), 10), C5="Drilling",MROUND(RANDBETWEEN(50,100), 10), C5="Grinding",MROUND(RANDBETWEEN(50,100), 10), C5="Boring",MROUND(RANDBETWEEN(50,100), 10), C5="Grooving",MROUND(RANDBETWEEN(100,250), 10), C5="Broaching",MROUND(RANDBETWEEN(200,400), 10), C5="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>890</v>
+        <v>930</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>12</v>
@@ -758,8 +773,11 @@
         <v>16</v>
       </c>
       <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -803,8 +821,11 @@
         <v>17</v>
       </c>
       <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -828,7 +849,7 @@
       </c>
       <c r="H7" s="2" cm="1">
         <f t="array" aca="1" ref="H7" ca="1">_xlfn.IFS( ((D7/(E7*(F7/(PI()*G7))))*60)&gt;1000, MROUND(RANDBETWEEN(800,1000),10), ((D7/(E7*(F7/(PI()*G7))))*60)&lt;100, MROUND(RANDBETWEEN(100,200),10), ((D7/(E7*(F7/(PI()*G7))))*60)&gt;100, MROUND((D7/(E7*(F7/(PI()*G7))))*60,10))</f>
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="I7" s="2" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_xlfn.IFS(C7="Milling",MROUND(RANDBETWEEN(300,500), 10), C7="Turning",MROUND(RANDBETWEEN(200,400), 10), C7="Drilling",MROUND(RANDBETWEEN(50,100), 10), C7="Grinding",MROUND(RANDBETWEEN(50,100), 10), C7="Boring",MROUND(RANDBETWEEN(50,100), 10), C7="Grooving",MROUND(RANDBETWEEN(100,250), 10), C7="Broaching",MROUND(RANDBETWEEN(200,400), 10), C7="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
@@ -836,7 +857,7 @@
       </c>
       <c r="J7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>35</v>
@@ -846,8 +867,11 @@
         <v>18</v>
       </c>
       <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -875,11 +899,11 @@
       </c>
       <c r="I8" s="2" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_xlfn.IFS(C8="Milling",MROUND(RANDBETWEEN(300,500), 10), C8="Turning",MROUND(RANDBETWEEN(200,400), 10), C8="Drilling",MROUND(RANDBETWEEN(50,100), 10), C8="Grinding",MROUND(RANDBETWEEN(50,100), 10), C8="Boring",MROUND(RANDBETWEEN(50,100), 10), C8="Grooving",MROUND(RANDBETWEEN(100,250), 10), C8="Broaching",MROUND(RANDBETWEEN(200,400), 10), C8="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>450</v>
+        <v>420</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>560</v>
+        <v>530</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="s">
@@ -889,8 +913,11 @@
         <v>18</v>
       </c>
       <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -918,11 +945,11 @@
       </c>
       <c r="I9" s="2" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_xlfn.IFS(C9="Milling",MROUND(RANDBETWEEN(300,500), 10), C9="Turning",MROUND(RANDBETWEEN(200,400), 10), C9="Drilling",MROUND(RANDBETWEEN(50,100), 10), C9="Grinding",MROUND(RANDBETWEEN(50,100), 10), C9="Boring",MROUND(RANDBETWEEN(50,100), 10), C9="Grooving",MROUND(RANDBETWEEN(100,250), 10), C9="Broaching",MROUND(RANDBETWEEN(200,400), 10), C9="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>770</v>
+        <v>780</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>27</v>
@@ -934,8 +961,11 @@
         <v>17</v>
       </c>
       <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -979,8 +1009,11 @@
         <v>16</v>
       </c>
       <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1008,11 +1041,11 @@
       </c>
       <c r="I11" s="2" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_xlfn.IFS(C11="Milling",MROUND(RANDBETWEEN(300,500), 10), C11="Turning",MROUND(RANDBETWEEN(200,400), 10), C11="Drilling",MROUND(RANDBETWEEN(50,100), 10), C11="Grinding",MROUND(RANDBETWEEN(50,100), 10), C11="Boring",MROUND(RANDBETWEEN(50,100), 10), C11="Grooving",MROUND(RANDBETWEEN(100,250), 10), C11="Broaching",MROUND(RANDBETWEEN(200,400), 10), C11="Honing",MROUND(RANDBETWEEN(50,100), 10))</f>
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>34</v>
@@ -1022,8 +1055,11 @@
         <v>18</v>
       </c>
       <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1031,7 +1067,7 @@
       <c r="L12" s="2"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="2"/>
@@ -1043,7 +1079,7 @@
       <c r="L13" s="2"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1053,7 +1089,7 @@
       <c r="L14" s="2"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1063,7 +1099,7 @@
       <c r="L15" s="2"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="2"/>

</xml_diff>